<commit_message>
Update Analysis Specifications and naming conventions for website 1.2.xlsx
</commit_message>
<xml_diff>
--- a/Content sources/Analysis Specifications and naming conventions for website 1.2.xlsx
+++ b/Content sources/Analysis Specifications and naming conventions for website 1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurice/Projects_Local/Github/thalassa-website/Content sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F823A3DF-2EFA-4E41-B63A-709BEB633AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5779C84D-BED7-1147-BB91-524A1A942B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="500" windowWidth="44000" windowHeight="40400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-47860" yWindow="9060" windowWidth="48780" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>Animation 2012 -22:  Where is growth erupting anually?  Is there a pattern?</t>
   </si>
   <si>
-    <t>Prescriptions Growth: % annual change of PPR1 in each LSOA</t>
-  </si>
-  <si>
     <t>Depression Growth: % annual change of DPR1 in each LSOA</t>
   </si>
   <si>
@@ -314,12 +311,6 @@
     <t>Prescriptions Prevalence and Growth = PPR</t>
   </si>
   <si>
-    <t>Prescriptions Prevalence: % of all GP registered patients with anti-depressant prescription in each LSOA</t>
-  </si>
-  <si>
-    <t>Animation 2012 -22:  How does presciption Prevalence  evolve and where are clusters of high or low depression forming?</t>
-  </si>
-  <si>
     <t>GWR using Depression Growth as the dependent variable and Depression Prevalence in the prior or current  year as the independent variable.  The objective is to see if eruptions of growth are more likely or less likely with high or low depresssion Prevalence (Implementation: LocalR2 with y: percentage_change x: est_qof_dep , need to see if previous year or current year)</t>
   </si>
   <si>
@@ -347,9 +338,6 @@
     <t>Depression Prevalence</t>
   </si>
   <si>
-    <t>Prescriptions Prevalence</t>
-  </si>
-  <si>
     <t>Items per Patient</t>
   </si>
   <si>
@@ -399,6 +387,18 @@
   </si>
   <si>
     <t>Depression Growth (Alternative Depression Growth Groups)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prescription Density (Prescription Items per All Patients in each LSOA)</t>
+  </si>
+  <si>
+    <t>Animation 2012 -22:  How does presciption Density  evolve and where are clusters of high or low presctription denisty forming?</t>
+  </si>
+  <si>
+    <t>Prescriptions Density Growth: % annual change of PPR1 in each LSOA</t>
+  </si>
+  <si>
+    <t>Prescriptions Density</t>
   </si>
 </sst>
 </file>
@@ -1266,12 +1266,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1294,9 +1288,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1364,12 +1355,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
@@ -1432,35 +1417,50 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2600,7 +2600,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2624,11 +2624,11 @@
   <sheetData>
     <row r="1" spans="1:20" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="59"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2658,30 +2658,30 @@
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="107" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="108" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="109" t="s">
+      <c r="D2" s="103" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="110" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="96" t="s">
+      <c r="F2" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="91" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>7</v>
@@ -2716,16 +2716,16 @@
     </row>
     <row r="3" spans="1:20" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="111" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="88" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="97"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="92"/>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
@@ -2744,20 +2744,20 @@
       <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="74" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="112" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="93" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="22" t="s">
@@ -2802,20 +2802,20 @@
     </row>
     <row r="5" spans="1:20" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="75" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="79" t="s">
+      <c r="B5" s="60"/>
+      <c r="C5" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="113" t="s">
+      <c r="F5" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="99" t="s">
+      <c r="G5" s="94" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="31" t="s">
@@ -2860,16 +2860,16 @@
     </row>
     <row r="6" spans="1:20" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="114" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="97"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="109" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="92"/>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -2886,20 +2886,20 @@
     </row>
     <row r="7" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="46"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="53" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="112" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="98" t="s">
+      <c r="F7" s="107" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="93" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="22" t="s">
@@ -2944,20 +2944,20 @@
     </row>
     <row r="8" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="79" t="s">
+      <c r="B8" s="62"/>
+      <c r="C8" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="115" t="s">
+      <c r="F8" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="95" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -3000,20 +3000,20 @@
     </row>
     <row r="9" spans="1:20" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="77" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="113" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="99" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="108" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="94" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="31" t="s">
@@ -3054,16 +3054,16 @@
     </row>
     <row r="10" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="114" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="97"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="92"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
@@ -3080,20 +3080,20 @@
     </row>
     <row r="11" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="57" t="s">
+      <c r="B11" s="63"/>
+      <c r="C11" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="101" t="s">
+      <c r="F11" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="96" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="38" t="s">
@@ -3138,20 +3138,20 @@
     </row>
     <row r="12" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="55" t="s">
+      <c r="B12" s="63"/>
+      <c r="C12" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="102"/>
+      <c r="F12" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="97"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -3170,20 +3170,20 @@
     </row>
     <row r="13" spans="1:20" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="55" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="102"/>
+      <c r="F13" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" s="97"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -3202,20 +3202,20 @@
     </row>
     <row r="14" spans="1:20" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="75" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="55" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="G14" s="102"/>
+      <c r="F14" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="97"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -3236,20 +3236,20 @@
     </row>
     <row r="15" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="78" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="80" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="G15" s="102"/>
+      <c r="G15" s="97"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -3265,25 +3265,25 @@
         <v>46</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="78" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="80" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" s="55" t="s">
+      <c r="B16" s="63"/>
+      <c r="C16" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="102"/>
+      <c r="F16" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="97"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -3304,20 +3304,20 @@
     </row>
     <row r="17" spans="1:20" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="116" t="s">
+      <c r="B17" s="63"/>
+      <c r="C17" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="117" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="118" t="s">
+      <c r="D17" s="112" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="103" t="s">
+      <c r="F17" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="98" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="39" t="s">
@@ -3337,19 +3337,19 @@
         <v>49</v>
       </c>
       <c r="T17" s="41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="120" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="97"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="127" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="128"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="92"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
@@ -3366,18 +3366,18 @@
     </row>
     <row r="19" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="42"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="122" t="s">
+      <c r="B19" s="87"/>
+      <c r="C19" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="67" t="s">
+      <c r="D19" s="67"/>
+      <c r="E19" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="123" t="s">
+      <c r="F19" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="119"/>
+      <c r="G19" s="114"/>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
@@ -3396,18 +3396,18 @@
     </row>
     <row r="20" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="124" t="s">
+      <c r="B20" s="88"/>
+      <c r="C20" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="68" t="s">
+      <c r="D20" s="68"/>
+      <c r="E20" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="125" t="s">
+      <c r="F20" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="102"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -3426,18 +3426,18 @@
     </row>
     <row r="21" spans="1:20" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="126" t="s">
+      <c r="B21" s="89"/>
+      <c r="C21" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="69" t="s">
+      <c r="D21" s="69"/>
+      <c r="E21" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="127" t="s">
+      <c r="F21" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="103"/>
+      <c r="G21" s="98"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
@@ -3454,18 +3454,18 @@
     </row>
     <row r="22" spans="1:20" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="116" t="s">
+      <c r="B22" s="89"/>
+      <c r="C22" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="128" t="s">
+      <c r="D22" s="70"/>
+      <c r="E22" s="122" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="129" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="103"/>
+      <c r="F22" s="123" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="98"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
@@ -3484,12 +3484,12 @@
     </row>
     <row r="23" spans="1:20" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="50" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="51"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="126"/>
       <c r="F23" s="25"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -3540,14 +3540,14 @@
       <c r="A25" s="15"/>
       <c r="B25" s="42"/>
       <c r="C25" s="48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="49" t="s">
         <v>61</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -3570,14 +3570,14 @@
       <c r="A26" s="15"/>
       <c r="B26" s="42"/>
       <c r="C26" s="48" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="49" t="s">
         <v>62</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -3610,12 +3610,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b11faa0b-7120-4a3e-99fd-301f7988c611" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="263f8bb8-dc0a-4d32-b4a4-20a8d684440c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3820,20 +3822,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b11faa0b-7120-4a3e-99fd-301f7988c611" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="263f8bb8-dc0a-4d32-b4a4-20a8d684440c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA7A291-6D4A-4614-BE37-CE695E75897A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47D4E9FB-1168-45CB-90B2-7D5B65099F07}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="263f8bb8-dc0a-4d32-b4a4-20a8d684440c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b11faa0b-7120-4a3e-99fd-301f7988c611"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3858,18 +3867,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47D4E9FB-1168-45CB-90B2-7D5B65099F07}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA7A291-6D4A-4614-BE37-CE695E75897A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="263f8bb8-dc0a-4d32-b4a4-20a8d684440c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b11faa0b-7120-4a3e-99fd-301f7988c611"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>